<commit_message>
Refactor - Ichthama component
</commit_message>
<xml_diff>
--- a/tabular/genus/ichthama-refseqs-side-data.xlsx
+++ b/tabular/genus/ichthama-refseqs-side-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/genus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DB2EEB-AFFF-0A4D-99B1-9E49DBBE5F1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2F908A-91B7-8849-9134-E87127AAB70A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22620" yWindow="1960" windowWidth="28040" windowHeight="17440" xr2:uid="{469403FE-80B6-3840-B15B-8B62EF5C2974}"/>
   </bookViews>
@@ -98,10 +98,10 @@
     <t>Ichthyic parvovirus isolate HMU-HKU</t>
   </si>
   <si>
-    <t>Icthamaparvovirus</t>
-  </si>
-  <si>
     <t>Tilapia</t>
+  </si>
+  <si>
+    <t>Ichthamaparvovirus</t>
   </si>
 </sst>
 </file>
@@ -510,7 +510,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,7 +578,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -590,7 +590,7 @@
         <v>17</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>13</v>

</xml_diff>